<commit_message>
class path and required file
</commit_message>
<xml_diff>
--- a/DynamicAutomation/src/main/resources/DATA/AutomationData.xlsx
+++ b/DynamicAutomation/src/main/resources/DATA/AutomationData.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>PunitRanjan</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Punit Ranjan2567339</t>
+  </si>
+  <si>
+    <t>Punit Ranjan25639174</t>
+  </si>
+  <si>
+    <t>Punit Ranjan25644748</t>
   </si>
 </sst>
 </file>
@@ -413,7 +419,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>